<commit_message>
Ajout liens 2024 de RWGPS
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1485B0-BD53-1849-9DC7-3096E679E7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2155AEA3-6A61-A341-B4BE-E03869E40989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68600" yWindow="1720" windowWidth="33480" windowHeight="20380" tabRatio="758" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68600" yWindow="1720" windowWidth="33480" windowHeight="20380" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="221">
   <si>
     <t>GPM</t>
   </si>
@@ -735,6 +735,9 @@
   </si>
   <si>
     <t>Virage à droite sur route 390</t>
+  </si>
+  <si>
+    <t>2024-01-07 : Étape 5 copiée de 2023 avant modif étape Senneterre. À valider.</t>
   </si>
 </sst>
 </file>
@@ -878,7 +881,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -895,6 +898,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1383,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AF60EC-7F0F-4893-B669-95F24DB4647E}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1447,6 +1453,16 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="14">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4036,8 +4052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308A417D-3276-6C45-809F-C6AB563D40A7}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Fin création tests pour validation GPX signalisation vs Excel
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2155AEA3-6A61-A341-B4BE-E03869E40989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A712DF-4ADC-3943-A475-E6A367EC2F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68600" yWindow="1720" windowWidth="33480" windowHeight="20380" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -1391,7 +1391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AF60EC-7F0F-4893-B669-95F24DB4647E}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -1476,7 +1476,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2347,7 +2347,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4616,16 +4616,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DA1B73-E162-C44F-BFAF-F0B7401711F0}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="83.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" customWidth="1"/>
@@ -4664,7 +4664,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <f t="shared" ref="C2:C20" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -4682,14 +4682,14 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="str">
-        <f>A2</f>
+        <f t="shared" ref="A3:A20" si="1">A2</f>
         <v>E6</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f t="shared" ref="C3:C20" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <f t="shared" si="0"/>
         <v>sign_02</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -4707,7 +4707,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="str">
-        <f t="shared" ref="A4:A28" si="1">A3</f>
+        <f t="shared" si="1"/>
         <v>E6</v>
       </c>
       <c r="B4" s="2">
@@ -5128,54 +5128,6 @@
       </c>
       <c r="G20" s="2" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" t="str">
-        <f t="shared" si="1"/>
-        <v>E6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" t="str">
-        <f t="shared" si="1"/>
-        <v>E6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" t="str">
-        <f t="shared" si="1"/>
-        <v>E6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" t="str">
-        <f t="shared" si="1"/>
-        <v>E6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" t="str">
-        <f t="shared" si="1"/>
-        <v>E6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" t="str">
-        <f t="shared" si="1"/>
-        <v>E6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" t="str">
-        <f t="shared" si="1"/>
-        <v>E6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" t="str">
-        <f t="shared" si="1"/>
-        <v>E6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout info signalisation etape 1
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9E1D86-14A6-8E4A-8808-A1335C351513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8128A045-2EE3-8E45-91E6-405472780270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="175">
   <si>
     <t>GPM</t>
   </si>
@@ -548,6 +548,57 @@
   </si>
   <si>
     <t xml:space="preserve">À MODIFIER </t>
+  </si>
+  <si>
+    <t>Voie ferrée oblique à la route</t>
+  </si>
+  <si>
+    <t>Contrôle policier, intersection route provinciale</t>
+  </si>
+  <si>
+    <t>Contrôle policier, intersection secteur Cadillac</t>
+  </si>
+  <si>
+    <t>Contrôle policier, intersection secteur Riviere-Heva</t>
+  </si>
+  <si>
+    <t>Contrôle policier, intersection secteur Ch. Lac Malartic</t>
+  </si>
+  <si>
+    <t>Voie ferrée perpendiculaire à la route et début du terre-plein</t>
+  </si>
+  <si>
+    <t>Voie ferrée oblique à la route - Malartic</t>
+  </si>
+  <si>
+    <t>Retressissment Ville de Malartic</t>
+  </si>
+  <si>
+    <t>sign_20</t>
+  </si>
+  <si>
+    <t>sign_21</t>
+  </si>
+  <si>
+    <t>sign_22</t>
+  </si>
+  <si>
+    <t>sign_23</t>
+  </si>
+  <si>
+    <t>Terre-Plein entrée rond point</t>
+  </si>
+  <si>
+    <t>sign_24</t>
+  </si>
+  <si>
+    <t>sign_25</t>
+  </si>
+  <si>
+    <t>Contrôle policier, intersection Boul. Barrette et Boul. Sabourin</t>
+  </si>
+  <si>
+    <t>Gestion dans rond-point - Signaleur et SQ pour traffic - tout à droite</t>
   </si>
 </sst>
 </file>
@@ -1600,21 +1651,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59035EEC-8A2E-CE47-A69A-0CAB24334359}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="62.5" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -1651,7 +1702,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
@@ -1664,74 +1715,601 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="10"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="10"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="10"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="10"/>
+      <c r="A6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="10"/>
+      <c r="A7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="10"/>
+      <c r="A8" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="10"/>
+      <c r="A9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="10"/>
+      <c r="A10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="10"/>
+      <c r="A11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="10"/>
+      <c r="A12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="10"/>
+      <c r="A13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="10"/>
+      <c r="A14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="10"/>
+      <c r="A15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" t="s">
+        <v>164</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="10"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="10"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="10"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="10"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="10"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="10"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="10"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="10"/>
+      <c r="A16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>169</v>
+      </c>
+      <c r="D24" t="s">
+        <v>170</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" s="10"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31" s="10"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A32" s="10"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="10"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="10"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="10"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="10"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="10"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38" s="10"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="10"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40" s="10"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -2019,7 +2597,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
-        <f t="shared" ref="A4:A10" si="1">A7</f>
+        <f t="shared" ref="A8:A10" si="1">A7</f>
         <v>0</v>
       </c>
       <c r="B8" s="5">
@@ -3169,7 +3747,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="str">
-        <f t="shared" ref="C2:C3" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <f t="shared" ref="C2" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">

</xml_diff>

<commit_message>
Ajout img signalisations etape 6 circuit urbain
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882ADF4E-9717-B54E-8E9D-2D4EB39AA86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EDF730-6E6D-1F4B-B1A6-A4B80995172E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="184">
   <si>
     <t>GPM</t>
   </si>
@@ -541,9 +541,6 @@
     <t>2024-01-07 : Étape 5 copiée de 2023 avant modif étape Senneterre. À valider.</t>
   </si>
   <si>
-    <t>Gestion du circuit urbain - Ville / CO</t>
-  </si>
-  <si>
     <t>TODO</t>
   </si>
   <si>
@@ -617,6 +614,18 @@
   </si>
   <si>
     <t>Retressissment Ville de Malartic - terre-plein av Hochelaga</t>
+  </si>
+  <si>
+    <t>Terre-plein Forest - Sabourin : tout à gauche</t>
+  </si>
+  <si>
+    <t>Bretelle Forest - Sabourin : tout à gauche - sens inverse</t>
+  </si>
+  <si>
+    <t>Bd Sabourin - Voie Est en sens inverse jusqu'à Des Pins</t>
+  </si>
+  <si>
+    <t>Intersection Des Pins direction voie Sud - séparation intersection en diagonale</t>
   </si>
 </sst>
 </file>
@@ -1671,7 +1680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59035EEC-8A2E-CE47-A69A-0CAB24334359}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -1743,7 +1752,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E3" t="s">
         <v>56</v>
@@ -1766,7 +1775,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
@@ -1789,7 +1798,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
@@ -1812,7 +1821,7 @@
         <v>111</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E6" t="s">
         <v>64</v>
@@ -1835,7 +1844,7 @@
         <v>112</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E7" t="s">
         <v>64</v>
@@ -1858,7 +1867,7 @@
         <v>113</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E8" t="s">
         <v>64</v>
@@ -1881,7 +1890,7 @@
         <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
@@ -1904,7 +1913,7 @@
         <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -1927,7 +1936,7 @@
         <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E11" t="s">
         <v>56</v>
@@ -1950,7 +1959,7 @@
         <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E12" t="s">
         <v>64</v>
@@ -1973,7 +1982,7 @@
         <v>102</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E13" t="s">
         <v>56</v>
@@ -1996,7 +2005,7 @@
         <v>96</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E14" t="s">
         <v>64</v>
@@ -2019,7 +2028,7 @@
         <v>97</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E15" t="s">
         <v>56</v>
@@ -2042,7 +2051,7 @@
         <v>98</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E16" t="s">
         <v>64</v>
@@ -2065,7 +2074,7 @@
         <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E17" t="s">
         <v>64</v>
@@ -2088,7 +2097,7 @@
         <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -2111,7 +2120,7 @@
         <v>116</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E19" t="s">
         <v>64</v>
@@ -2134,7 +2143,7 @@
         <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E20" t="s">
         <v>64</v>
@@ -2154,10 +2163,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
@@ -2177,10 +2186,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E22" t="s">
         <v>64</v>
@@ -2200,10 +2209,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E23" t="s">
         <v>64</v>
@@ -2223,10 +2232,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" t="s">
         <v>165</v>
-      </c>
-      <c r="D24" t="s">
-        <v>166</v>
       </c>
       <c r="E24" t="s">
         <v>56</v>
@@ -2246,7 +2255,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D25" t="s">
         <v>150</v>
@@ -2269,10 +2278,10 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" t="s">
         <v>168</v>
-      </c>
-      <c r="D26" t="s">
-        <v>169</v>
       </c>
       <c r="E26" t="s">
         <v>64</v>
@@ -2413,7 +2422,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
@@ -2801,7 +2810,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
@@ -3719,8 +3728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DA1B73-E162-C44F-BFAF-F0B7401711F0}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3758,56 +3767,119 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="str">
-        <f t="shared" ref="C2" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
-        <v>sign_01</v>
+      <c r="C2" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B3" s="2"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B4" s="2"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B5" s="2"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B6" s="2"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7" s="2"/>
@@ -3919,7 +3991,7 @@
           <x14:formula1>
             <xm:f>Lexique!$F$2:$F$17</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G18</xm:sqref>
+          <xm:sqref>G7:G18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3981,7 +4053,7 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Compil guide organisateur - etape 3
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EDF730-6E6D-1F4B-B1A6-A4B80995172E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74BF35F-8D8D-BC4A-99FC-20D631308DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="560" windowWidth="34020" windowHeight="28180" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="192">
   <si>
     <t>GPM</t>
   </si>
@@ -430,21 +430,6 @@
     <t>sign_19</t>
   </si>
   <si>
-    <t>Rampe de départ</t>
-  </si>
-  <si>
-    <t>Section fermée - départ</t>
-  </si>
-  <si>
-    <t>Installations ligne arrivée</t>
-  </si>
-  <si>
-    <t>Zone décélération et sortie</t>
-  </si>
-  <si>
-    <t>Déviation des voitures équipe suiveuse - 3e &amp; 1ere</t>
-  </si>
-  <si>
     <t>E6</t>
   </si>
   <si>
@@ -626,6 +611,45 @@
   </si>
   <si>
     <t>Intersection Des Pins direction voie Sud - séparation intersection en diagonale</t>
+  </si>
+  <si>
+    <t>Rampe de départ - voir croquis complet</t>
+  </si>
+  <si>
+    <t>Virage gauche - rue Allard - 2 sens - séparation</t>
+  </si>
+  <si>
+    <t>Virage droite - École - séparation 2 sens</t>
+  </si>
+  <si>
+    <t>Entrée - Sortie Moto suiveuse</t>
+  </si>
+  <si>
+    <t>Terre-plein - séparation voies Dennison - tout à droite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retour sur une seule voie </t>
+  </si>
+  <si>
+    <t>Virage à gauche - rue Self - 2 sens</t>
+  </si>
+  <si>
+    <t>Terre-plein - Self &amp; 7e - 2 sens dans la voie Sud</t>
+  </si>
+  <si>
+    <t>Intersection double sens Des Pins - Sabourin</t>
+  </si>
+  <si>
+    <t>Entrée - Sortie Stationnement pour demi Tour</t>
+  </si>
+  <si>
+    <t>Demi-Tour -- fond du stationnement roulotte</t>
+  </si>
+  <si>
+    <t>Terre-plein retour sur Rue Self</t>
+  </si>
+  <si>
+    <t>Zone décélération à protéger (voie de traverse des voitures)</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1374,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1483,7 +1507,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>56</v>
@@ -1681,7 +1705,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1729,7 +1753,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
@@ -1752,7 +1776,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E3" t="s">
         <v>56</v>
@@ -1775,7 +1799,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
@@ -1798,7 +1822,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
@@ -1821,7 +1845,7 @@
         <v>111</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E6" t="s">
         <v>64</v>
@@ -1844,7 +1868,7 @@
         <v>112</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E7" t="s">
         <v>64</v>
@@ -1867,7 +1891,7 @@
         <v>113</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E8" t="s">
         <v>64</v>
@@ -1890,7 +1914,7 @@
         <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
@@ -1913,7 +1937,7 @@
         <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -1936,7 +1960,7 @@
         <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E11" t="s">
         <v>56</v>
@@ -1959,7 +1983,7 @@
         <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E12" t="s">
         <v>64</v>
@@ -1982,7 +2006,7 @@
         <v>102</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E13" t="s">
         <v>56</v>
@@ -2005,7 +2029,7 @@
         <v>96</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E14" t="s">
         <v>64</v>
@@ -2028,7 +2052,7 @@
         <v>97</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E15" t="s">
         <v>56</v>
@@ -2051,7 +2075,7 @@
         <v>98</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E16" t="s">
         <v>64</v>
@@ -2074,7 +2098,7 @@
         <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E17" t="s">
         <v>64</v>
@@ -2097,7 +2121,7 @@
         <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -2120,7 +2144,7 @@
         <v>116</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E19" t="s">
         <v>64</v>
@@ -2143,7 +2167,7 @@
         <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E20" t="s">
         <v>64</v>
@@ -2163,10 +2187,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D21" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
@@ -2186,10 +2210,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E22" t="s">
         <v>64</v>
@@ -2209,10 +2233,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E23" t="s">
         <v>64</v>
@@ -2232,10 +2256,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D24" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E24" t="s">
         <v>56</v>
@@ -2255,10 +2279,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D25" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E25" t="s">
         <v>64</v>
@@ -2278,10 +2302,10 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D26" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E26" t="s">
         <v>64</v>
@@ -2422,7 +2446,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
@@ -2513,21 +2537,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB129F3F-5845-E94C-BB9B-41541692CC0D}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="62.5" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.5" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -2557,7 +2581,7 @@
       <c r="A2" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="str">
@@ -2565,7 +2589,7 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>118</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
         <v>65</v>
@@ -2573,119 +2597,199 @@
       <c r="F2" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>63</v>
+      <c r="G2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" t="str">
+      <c r="A3" s="8" t="str">
         <f>A2</f>
         <v>E3</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f t="shared" ref="C3:C10" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <f t="shared" ref="C3:C4" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
         <v>sign_02</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="8" t="str">
+        <f t="shared" ref="A4:A15" si="1">A3</f>
+        <v>E3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_03</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>E3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <f t="shared" ref="C5:C15" si="2">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B5,"0#"))</f>
+        <v>sign_04</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>E3</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>sign_05</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>E3</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>sign_06</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <f t="shared" ref="A8:A10" si="1">A7</f>
-        <v>0</v>
-      </c>
-      <c r="B8" s="5">
-        <v>90</v>
+      <c r="A8" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>E3</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_90</v>
+        <f t="shared" si="2"/>
+        <v>sign_07</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>120</v>
+        <v>185</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>E3</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>sign_08</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="B9" s="5">
-        <v>91</v>
-      </c>
-      <c r="C9" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_91</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="B10" s="5">
-        <v>92</v>
+        <v>E3</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
       </c>
       <c r="C10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_92</v>
+        <f t="shared" si="2"/>
+        <v>sign_09</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>122</v>
+        <v>187</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -2694,31 +2798,135 @@
         <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>E3</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>sign_10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="A12" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>E3</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>sign_11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="A13" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>E3</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>sign_12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="A14" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>E3</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>sign_13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="A15" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>E3</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>sign_14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.15">
@@ -2728,6 +2936,42 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2739,19 +2983,19 @@
           <x14:formula1>
             <xm:f>Lexique!$D$2:$D$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E10</xm:sqref>
+          <xm:sqref>E2:E27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CADB21EB-5FBA-F948-91A8-13DA27ECCDDC}">
           <x14:formula1>
             <xm:f>Lexique!$E$2:$E$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F10</xm:sqref>
+          <xm:sqref>F2:F27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{446A4710-3B5A-9247-B67D-D204A01F91E2}">
           <x14:formula1>
             <xm:f>Lexique!$F$2:$F$13</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G10</xm:sqref>
+          <xm:sqref>G2:G27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2801,7 +3045,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -2810,7 +3054,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
@@ -2824,7 +3068,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -2833,7 +3077,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>64</v>
@@ -2847,7 +3091,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -2856,7 +3100,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>56</v>
@@ -2870,7 +3114,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -2879,7 +3123,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>56</v>
@@ -2893,7 +3137,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -2902,7 +3146,7 @@
         <v>111</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>56</v>
@@ -2916,7 +3160,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -2925,7 +3169,7 @@
         <v>112</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>64</v>
@@ -2939,7 +3183,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -2948,7 +3192,7 @@
         <v>113</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>65</v>
@@ -2957,12 +3201,12 @@
         <v>73</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -2971,7 +3215,7 @@
         <v>95</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>65</v>
@@ -2980,12 +3224,12 @@
         <v>73</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -2994,7 +3238,7 @@
         <v>101</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>64</v>
@@ -3003,12 +3247,12 @@
         <v>74</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -3017,7 +3261,7 @@
         <v>114</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>64</v>
@@ -3026,12 +3270,12 @@
         <v>74</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -3040,7 +3284,7 @@
         <v>115</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>64</v>
@@ -3054,7 +3298,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -3063,7 +3307,7 @@
         <v>102</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>56</v>
@@ -3077,7 +3321,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -3086,7 +3330,7 @@
         <v>96</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>64</v>
@@ -3100,7 +3344,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -3109,7 +3353,7 @@
         <v>97</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>64</v>
@@ -3123,7 +3367,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -3132,7 +3376,7 @@
         <v>98</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>64</v>
@@ -3202,7 +3446,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -3211,7 +3455,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
@@ -3225,7 +3469,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -3234,7 +3478,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>56</v>
@@ -3248,7 +3492,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -3257,7 +3501,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>64</v>
@@ -3271,7 +3515,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -3294,7 +3538,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -3317,7 +3561,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -3340,7 +3584,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -3363,7 +3607,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -3386,7 +3630,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -3395,7 +3639,7 @@
         <v>101</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>56</v>
@@ -3409,7 +3653,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -3418,7 +3662,7 @@
         <v>114</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>65</v>
@@ -3427,12 +3671,12 @@
         <v>73</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -3441,7 +3685,7 @@
         <v>115</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>65</v>
@@ -3450,12 +3694,12 @@
         <v>73</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -3464,7 +3708,7 @@
         <v>102</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>64</v>
@@ -3478,7 +3722,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -3501,7 +3745,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -3510,7 +3754,7 @@
         <v>97</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>64</v>
@@ -3524,7 +3768,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -3533,7 +3777,7 @@
         <v>98</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>64</v>
@@ -3547,7 +3791,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
@@ -3556,7 +3800,7 @@
         <v>99</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>64</v>
@@ -3570,7 +3814,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -3579,7 +3823,7 @@
         <v>100</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>64</v>
@@ -3593,7 +3837,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
@@ -3602,7 +3846,7 @@
         <v>116</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>64</v>
@@ -3616,7 +3860,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
@@ -3625,7 +3869,7 @@
         <v>117</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>64</v>
@@ -3639,16 +3883,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B21" s="2">
         <v>50</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>64</v>
@@ -3662,16 +3906,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B22" s="2">
         <v>51</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>64</v>
@@ -3685,16 +3929,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B23" s="2">
         <v>60</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>56</v>
@@ -3728,7 +3972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DA1B73-E162-C44F-BFAF-F0B7401711F0}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -3768,7 +4012,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -3777,7 +4021,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
@@ -3791,7 +4035,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -3800,7 +4044,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>65</v>
@@ -3814,7 +4058,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -3823,7 +4067,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>65</v>
@@ -3837,7 +4081,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -3846,7 +4090,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>64</v>
@@ -3860,7 +4104,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -3869,7 +4113,7 @@
         <v>111</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>64</v>
@@ -4053,7 +4297,7 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Compil guide organisateur post signalisation etape 4
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74BF35F-8D8D-BC4A-99FC-20D631308DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF6119E-F679-204B-AC6B-5322461F87AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="560" windowWidth="34020" windowHeight="28180" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="540" windowWidth="34020" windowHeight="28180" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="199">
   <si>
     <t>GPM</t>
   </si>
@@ -493,12 +493,6 @@
     <t>Point de croisement de la course - Cadillac</t>
   </si>
   <si>
-    <t>Contrôle Traffic 117</t>
-  </si>
-  <si>
-    <t>Bollards vidange roulottes - signalisation pour protéger - Ville de RN</t>
-  </si>
-  <si>
     <t>Rétrécicement troittoir - signalisation pour protéger - Ville de RN</t>
   </si>
   <si>
@@ -514,24 +508,12 @@
     <t>Gestion dans rond-point - Signaleur et SQ pour traffic</t>
   </si>
   <si>
-    <t>Virage gauche - Harricana</t>
-  </si>
-  <si>
-    <t>Virage gauche - 4e avenue</t>
-  </si>
-  <si>
-    <t>Déviation caravane - des Érables</t>
-  </si>
-  <si>
     <t>2024-01-07 : Étape 5 copiée de 2023 avant modif étape Senneterre. À valider.</t>
   </si>
   <si>
     <t>TODO</t>
   </si>
   <si>
-    <t xml:space="preserve">À MODIFIER </t>
-  </si>
-  <si>
     <t>Voie ferrée oblique à la route</t>
   </si>
   <si>
@@ -650,6 +632,45 @@
   </si>
   <si>
     <t>Zone décélération à protéger (voie de traverse des voitures)</t>
+  </si>
+  <si>
+    <t>Terre-plein</t>
+  </si>
+  <si>
+    <t>Légèrement à droite - Ch Lac Mourier</t>
+  </si>
+  <si>
+    <t>Légèrement à droite - Rivière-Héva &amp; Intersection Amos</t>
+  </si>
+  <si>
+    <t>Virage gauche - Rue La Sarre</t>
+  </si>
+  <si>
+    <t>Virage gauche - 117 / Royale</t>
+  </si>
+  <si>
+    <t>Contrôle Traffic 117 - Virage gauche rue Principale</t>
+  </si>
+  <si>
+    <t>Rétrécicement bollard protextion - signalisation pour protéger - Ville de RN</t>
+  </si>
+  <si>
+    <t>Rétrécicement troittoir rue des Pins - signalisation pour protéger</t>
+  </si>
+  <si>
+    <t>Voie ferré / Terre-plein - tous à droite</t>
+  </si>
+  <si>
+    <t>Intersection rue La Salle - tout droit</t>
+  </si>
+  <si>
+    <t>Virage en "S" vers Avenue d'Abitibi</t>
+  </si>
+  <si>
+    <t>Virage final à gauche - rue de la Paix</t>
+  </si>
+  <si>
+    <t>Zone décélération jsuqu'à rue La Sarre</t>
   </si>
 </sst>
 </file>
@@ -1374,7 +1395,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1726,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B16"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1753,7 +1774,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
@@ -1776,7 +1797,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E3" t="s">
         <v>56</v>
@@ -1799,7 +1820,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
@@ -1822,7 +1843,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
@@ -1845,7 +1866,7 @@
         <v>111</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E6" t="s">
         <v>64</v>
@@ -1868,7 +1889,7 @@
         <v>112</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E7" t="s">
         <v>64</v>
@@ -1891,7 +1912,7 @@
         <v>113</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E8" t="s">
         <v>64</v>
@@ -1914,7 +1935,7 @@
         <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
@@ -1937,7 +1958,7 @@
         <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -1960,7 +1981,7 @@
         <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E11" t="s">
         <v>56</v>
@@ -1983,7 +2004,7 @@
         <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E12" t="s">
         <v>64</v>
@@ -2006,7 +2027,7 @@
         <v>102</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E13" t="s">
         <v>56</v>
@@ -2029,7 +2050,7 @@
         <v>96</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E14" t="s">
         <v>64</v>
@@ -2052,7 +2073,7 @@
         <v>97</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E15" t="s">
         <v>56</v>
@@ -2075,7 +2096,7 @@
         <v>98</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E16" t="s">
         <v>64</v>
@@ -2098,7 +2119,7 @@
         <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E17" t="s">
         <v>64</v>
@@ -2121,7 +2142,7 @@
         <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -2144,7 +2165,7 @@
         <v>116</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E19" t="s">
         <v>64</v>
@@ -2167,7 +2188,7 @@
         <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E20" t="s">
         <v>64</v>
@@ -2187,10 +2208,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
@@ -2210,10 +2231,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E22" t="s">
         <v>64</v>
@@ -2233,10 +2254,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E23" t="s">
         <v>64</v>
@@ -2256,10 +2277,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D24" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E24" t="s">
         <v>56</v>
@@ -2279,10 +2300,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E25" t="s">
         <v>64</v>
@@ -2302,10 +2323,10 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D26" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E26" t="s">
         <v>64</v>
@@ -2446,7 +2467,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
@@ -2539,8 +2560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB129F3F-5845-E94C-BB9B-41541692CC0D}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2589,7 +2610,7 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E2" t="s">
         <v>65</v>
@@ -2614,7 +2635,7 @@
         <v>sign_02</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E3" t="s">
         <v>64</v>
@@ -2639,7 +2660,7 @@
         <v>sign_03</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E4" t="s">
         <v>65</v>
@@ -2664,7 +2685,7 @@
         <v>sign_04</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
@@ -2689,7 +2710,7 @@
         <v>sign_05</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E6" t="s">
         <v>65</v>
@@ -2714,7 +2735,7 @@
         <v>sign_06</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E7" t="s">
         <v>65</v>
@@ -2739,7 +2760,7 @@
         <v>sign_07</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E8" t="s">
         <v>64</v>
@@ -2764,7 +2785,7 @@
         <v>sign_08</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
@@ -2789,7 +2810,7 @@
         <v>sign_09</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -2814,7 +2835,7 @@
         <v>sign_10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E11" t="s">
         <v>64</v>
@@ -2839,7 +2860,7 @@
         <v>sign_11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E12" t="s">
         <v>64</v>
@@ -2864,7 +2885,7 @@
         <v>sign_12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E13" t="s">
         <v>64</v>
@@ -2889,7 +2910,7 @@
         <v>sign_13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E14" t="s">
         <v>65</v>
@@ -2914,7 +2935,7 @@
         <v>sign_14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E15" t="s">
         <v>64</v>
@@ -3005,16 +3026,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F06BA10-C7CB-D34A-A68E-94110B0F7625}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="62.5" customWidth="1"/>
     <col min="5" max="7" width="15.6640625" customWidth="1"/>
@@ -3050,355 +3071,621 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>92</v>
+      <c r="C2" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="13" t="s">
         <v>134</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>93</v>
+      <c r="C3" s="2" t="str">
+        <f t="shared" ref="C3:C24" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <v>sign_02</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>66</v>
+      <c r="G3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="13" t="s">
         <v>134</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>94</v>
+      <c r="C4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_03</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>136</v>
+        <v>186</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="13" t="s">
         <v>134</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>110</v>
+      <c r="C5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_04</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>137</v>
+        <v>186</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="2">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_06</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="2">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_07</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="2">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="2">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_09</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="2">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="B9" s="2">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="2">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_05</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="2">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="2">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_14</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="2">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_15</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="13" t="str">
+        <f>A14</f>
+        <v>E4</v>
+      </c>
+      <c r="B15" s="5">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_08</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="13" t="str">
+        <f t="shared" ref="A16:A24" si="1">A15</f>
+        <v>E4</v>
+      </c>
+      <c r="B16" s="5">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>187</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="B18">
+        <v>21</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>143</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="B19">
+        <v>22</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_22</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E19" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F19" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="2">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="G19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="B20">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_23</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="B21">
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_24</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="B22">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_25</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="B23">
+        <v>26</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_26</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="B24">
+        <v>27</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_27</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E24" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F24" t="s">
         <v>73</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="2">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="2">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B12" s="2">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="G24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B13" s="2">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B14" s="2">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="2">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B16" s="2">
-        <v>15</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="13"/>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" s="13"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" s="13"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C6514F4A-BD79-DB46-A0BE-57501B73CBDD}">
+          <x14:formula1>
+            <xm:f>Lexique!$F$2:$F$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>G8 G3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{463BCA35-24F0-AE4C-9B9D-BD2295FAB2D2}">
+          <x14:formula1>
+            <xm:f>Lexique!$E$2:$E$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>F8 F3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCABF94A-CF6E-0142-A54D-4679177E7DC0}">
+          <x14:formula1>
+            <xm:f>Lexique!$D$2:$D$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>E8 E3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B510EDD3-1D60-2C4F-BC8F-8A16F0CAE8D8}">
+          <x14:formula1>
+            <xm:f>Lexique!$F$2:$F$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>G18:G41</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4754FE9-959E-5446-A32D-C448446ADFA1}">
+          <x14:formula1>
+            <xm:f>Lexique!$E$2:$E$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>F18:F41</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{55D5426C-BF6C-674D-B316-A5FC9600E4BB}">
+          <x14:formula1>
+            <xm:f>Lexique!$D$2:$D$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>E18:E41</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3972,7 +4259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DA1B73-E162-C44F-BFAF-F0B7401711F0}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4021,7 +4308,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
@@ -4044,7 +4331,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>65</v>
@@ -4067,7 +4354,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>65</v>
@@ -4090,7 +4377,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>64</v>
@@ -4113,7 +4400,7 @@
         <v>111</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>64</v>
@@ -4297,7 +4584,7 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Ajout déviation caravane etape 3
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF6119E-F679-204B-AC6B-5322461F87AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0144855E-A3FE-F944-92D2-89CE574F636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="540" windowWidth="34020" windowHeight="28180" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="540" windowWidth="34020" windowHeight="28180" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="200">
   <si>
     <t>GPM</t>
   </si>
@@ -671,6 +671,9 @@
   </si>
   <si>
     <t>Zone décélération jsuqu'à rue La Sarre</t>
+  </si>
+  <si>
+    <t>Zone déviation voitures suiveuses</t>
   </si>
 </sst>
 </file>
@@ -2560,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB129F3F-5845-E94C-BB9B-41541692CC0D}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2649,7 +2652,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="str">
-        <f t="shared" ref="A4:A15" si="1">A3</f>
+        <f t="shared" ref="A4:A16" si="1">A3</f>
         <v>E3</v>
       </c>
       <c r="B4">
@@ -2928,14 +2931,14 @@
         <v>E3</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>sign_14</v>
+        <v>sign_15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="E15" t="s">
         <v>64</v>
@@ -2948,7 +2951,29 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C16" s="5"/>
+      <c r="A16" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>E3</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" s="5" t="str">
+        <f t="shared" ref="C16" si="3">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B16,"0#"))</f>
+        <v>sign_14</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B17" s="5"/>
@@ -4259,7 +4284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DA1B73-E162-C44F-BFAF-F0B7401711F0}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajout éléments signalisation E2 et E7
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82B1126-1B51-9246-9E38-E4090BDB7AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EFF476-D64C-5848-9B65-BC1A68CB4526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6980" yWindow="1180" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="221">
   <si>
     <t>GPM</t>
   </si>
@@ -511,9 +511,6 @@
     <t>2024-01-07 : Étape 5 copiée de 2023 avant modif étape Senneterre. À valider.</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>Voie ferrée oblique à la route</t>
   </si>
   <si>
@@ -674,6 +671,72 @@
   </si>
   <si>
     <t>Zone décélération jsuqu'à rue Hochelaga</t>
+  </si>
+  <si>
+    <t>Voie ferrée</t>
+  </si>
+  <si>
+    <t>Terre-plein après voie ferrée</t>
+  </si>
+  <si>
+    <t>Terre-plein, tout à droite (devant Centre du camping)</t>
+  </si>
+  <si>
+    <t>Terre-plein, tout à droite (devant AIM)</t>
+  </si>
+  <si>
+    <t>Terre-plein, tout à droite (devant pneu GBM)</t>
+  </si>
+  <si>
+    <t>Virage gauche,Contrôle policier, intersection route provinciale</t>
+  </si>
+  <si>
+    <t>Voie ferrée à angle</t>
+  </si>
+  <si>
+    <t>Contrôle policier, virage à droite sur route provinciale 386</t>
+  </si>
+  <si>
+    <t>Terre-Plein (Barraute, virage à gauche)</t>
+  </si>
+  <si>
+    <t>Terre-plein blvd JJ Cossette (tout à droite, après intersection du Portage)</t>
+  </si>
+  <si>
+    <t>Entrée carrefour giratoire 7e rue &amp; 117, (tout à droite)</t>
+  </si>
+  <si>
+    <t>Terre-plein intersection 7e &amp; 7e (tout à droite)</t>
+  </si>
+  <si>
+    <t>sign_32</t>
+  </si>
+  <si>
+    <t>sign_33</t>
+  </si>
+  <si>
+    <t>Entrée dans rond point - terre-plein</t>
+  </si>
+  <si>
+    <t>Terre-plein, tout à droite (devant Mazda)</t>
+  </si>
+  <si>
+    <t>sign_34</t>
+  </si>
+  <si>
+    <t>Terre-plein, tout à droite (devant cimetière)</t>
+  </si>
+  <si>
+    <t>Virage à gauche sur 4e rue ouest</t>
+  </si>
+  <si>
+    <t>Virage à droite par la bretelle</t>
+  </si>
+  <si>
+    <t>Contrôle policier, intersection route provinciale, virage à droite sur route 117</t>
+  </si>
+  <si>
+    <t>Terre-plein, tout à gauche et prendre première sortie à gauche</t>
   </si>
 </sst>
 </file>
@@ -1800,7 +1863,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E3" t="s">
         <v>56</v>
@@ -1823,7 +1886,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
@@ -1846,7 +1909,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
@@ -1869,7 +1932,7 @@
         <v>111</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E6" t="s">
         <v>64</v>
@@ -1892,7 +1955,7 @@
         <v>112</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E7" t="s">
         <v>64</v>
@@ -1915,7 +1978,7 @@
         <v>113</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E8" t="s">
         <v>64</v>
@@ -1938,7 +2001,7 @@
         <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
@@ -1961,7 +2024,7 @@
         <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -1984,7 +2047,7 @@
         <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
         <v>56</v>
@@ -2007,7 +2070,7 @@
         <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
         <v>64</v>
@@ -2030,7 +2093,7 @@
         <v>102</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E13" t="s">
         <v>56</v>
@@ -2053,7 +2116,7 @@
         <v>96</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E14" t="s">
         <v>64</v>
@@ -2076,7 +2139,7 @@
         <v>97</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E15" t="s">
         <v>56</v>
@@ -2099,7 +2162,7 @@
         <v>98</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E16" t="s">
         <v>64</v>
@@ -2122,7 +2185,7 @@
         <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E17" t="s">
         <v>64</v>
@@ -2145,7 +2208,7 @@
         <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -2168,7 +2231,7 @@
         <v>116</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E19" t="s">
         <v>64</v>
@@ -2191,7 +2254,7 @@
         <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E20" t="s">
         <v>64</v>
@@ -2211,10 +2274,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
@@ -2234,10 +2297,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E22" t="s">
         <v>64</v>
@@ -2257,10 +2320,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E23" t="s">
         <v>64</v>
@@ -2280,10 +2343,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" t="s">
         <v>153</v>
-      </c>
-      <c r="D24" t="s">
-        <v>154</v>
       </c>
       <c r="E24" t="s">
         <v>56</v>
@@ -2303,7 +2366,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D25" t="s">
         <v>143</v>
@@ -2326,10 +2389,10 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" t="s">
         <v>156</v>
-      </c>
-      <c r="D26" t="s">
-        <v>157</v>
       </c>
       <c r="E26" t="s">
         <v>64</v>
@@ -2419,10 +2482,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4800E175-391C-4882-AD71-91732BA4C7F2}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2470,63 +2533,546 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>145</v>
+        <v>199</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
         <v>53</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="2"/>
-      <c r="G6" s="11"/>
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="2"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="G8" s="11"/>
+      <c r="A8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="2">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" t="s">
+        <v>202</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" t="s">
+        <v>206</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>207</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="5">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="5">
+        <v>14</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="5">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="5">
+        <v>16</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="5">
+        <v>17</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="5">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" t="s">
+        <v>209</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="5">
+        <v>19</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" t="s">
+        <v>199</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D25" t="s">
+        <v>210</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -2534,24 +3080,24 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7BB46DD1-CE67-8840-86C9-A7B4DD4EA804}">
           <x14:formula1>
             <xm:f>Lexique!$D$2:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>E14:E1048576 E2:E13</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B2F24BC-BBE5-3242-8C11-39321438202A}">
           <x14:formula1>
             <xm:f>Lexique!$E$2:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F14:F1048576 F2:F13</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2AB93EB3-1866-E243-98C3-B11D12762F37}">
           <x14:formula1>
             <xm:f>Lexique!$F$2:$F$17</xm:f>
           </x14:formula1>
-          <xm:sqref>G14:G1048576 G2:G13</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2613,7 +3159,7 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E2" t="s">
         <v>65</v>
@@ -2638,7 +3184,7 @@
         <v>sign_02</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E3" t="s">
         <v>64</v>
@@ -2663,7 +3209,7 @@
         <v>sign_03</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E4" t="s">
         <v>65</v>
@@ -2688,7 +3234,7 @@
         <v>sign_04</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
@@ -2713,7 +3259,7 @@
         <v>sign_05</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E6" t="s">
         <v>65</v>
@@ -2738,7 +3284,7 @@
         <v>sign_06</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E7" t="s">
         <v>65</v>
@@ -2763,7 +3309,7 @@
         <v>sign_07</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E8" t="s">
         <v>64</v>
@@ -2788,7 +3334,7 @@
         <v>sign_08</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
@@ -2813,7 +3359,7 @@
         <v>sign_09</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -2838,7 +3384,7 @@
         <v>sign_10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E11" t="s">
         <v>64</v>
@@ -2863,7 +3409,7 @@
         <v>sign_11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E12" t="s">
         <v>64</v>
@@ -2888,7 +3434,7 @@
         <v>sign_12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E13" t="s">
         <v>64</v>
@@ -2913,7 +3459,7 @@
         <v>sign_13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E14" t="s">
         <v>65</v>
@@ -2938,7 +3484,7 @@
         <v>sign_15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E15" t="s">
         <v>64</v>
@@ -2963,7 +3509,7 @@
         <v>sign_14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E16" t="s">
         <v>64</v>
@@ -3053,7 +3599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F06BA10-C7CB-D34A-A68E-94110B0F7625}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -3101,7 +3647,7 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>65</v>
@@ -3125,7 +3671,7 @@
         <v>sign_02</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E3" t="s">
         <v>64</v>
@@ -3149,7 +3695,7 @@
         <v>sign_03</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>64</v>
@@ -3173,7 +3719,7 @@
         <v>sign_04</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>64</v>
@@ -3293,7 +3839,7 @@
         <v>sign_12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -3317,7 +3863,7 @@
         <v>sign_05</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>65</v>
@@ -3414,7 +3960,7 @@
         <v>sign_08</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E15" t="s">
         <v>64</v>
@@ -3439,7 +3985,7 @@
         <v>sign_16</v>
       </c>
       <c r="D16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E16" t="s">
         <v>56</v>
@@ -3514,7 +4060,7 @@
         <v>sign_22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E19" t="s">
         <v>65</v>
@@ -3539,7 +4085,7 @@
         <v>sign_23</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E20" t="s">
         <v>64</v>
@@ -3564,7 +4110,7 @@
         <v>sign_24</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
@@ -3589,7 +4135,7 @@
         <v>sign_25</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E22" t="s">
         <v>64</v>
@@ -3614,7 +4160,7 @@
         <v>sign_26</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E23" t="s">
         <v>64</v>
@@ -3639,7 +4185,7 @@
         <v>sign_27</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E24" t="s">
         <v>65</v>
@@ -4333,7 +4879,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
@@ -4356,7 +4902,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>65</v>
@@ -4379,7 +4925,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>65</v>
@@ -4402,7 +4948,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>64</v>
@@ -4425,7 +4971,7 @@
         <v>111</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>64</v>
@@ -4559,8 +5105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F8F1C6-7AEF-9949-BBA2-37380A45C53E}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4604,12 +5150,11 @@
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
-        <v>sign_01</v>
+      <c r="C2" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
@@ -4622,44 +5167,234 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="5">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="5">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="5">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="5">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="5">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="A12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="5">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>

</xml_diff>

<commit_message>
E1 - cleanup Malartic
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinebeausoleil/Documents/TourAbitibi/Guide/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EFF476-D64C-5848-9B65-BC1A68CB4526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A32B74-0BF6-9B47-B2D1-068F9BF51543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="1180" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="172">
   <si>
     <t>GPM</t>
   </si>
@@ -430,6 +430,21 @@
     <t>sign_19</t>
   </si>
   <si>
+    <t>Rampe de départ</t>
+  </si>
+  <si>
+    <t>Section fermée - départ</t>
+  </si>
+  <si>
+    <t>Installations ligne arrivée</t>
+  </si>
+  <si>
+    <t>Zone décélération et sortie</t>
+  </si>
+  <si>
+    <t>Déviation des voitures équipe suiveuse - 3e &amp; 1ere</t>
+  </si>
+  <si>
     <t>E6</t>
   </si>
   <si>
@@ -493,6 +508,12 @@
     <t>Point de croisement de la course - Cadillac</t>
   </si>
   <si>
+    <t>Contrôle Traffic 117</t>
+  </si>
+  <si>
+    <t>Bollards vidange roulottes - signalisation pour protéger - Ville de RN</t>
+  </si>
+  <si>
     <t>Rétrécicement troittoir - signalisation pour protéger - Ville de RN</t>
   </si>
   <si>
@@ -508,30 +529,51 @@
     <t>Gestion dans rond-point - Signaleur et SQ pour traffic</t>
   </si>
   <si>
+    <t>Virage gauche - Harricana</t>
+  </si>
+  <si>
+    <t>Virage gauche - 4e avenue</t>
+  </si>
+  <si>
+    <t>Déviation caravane - des Érables</t>
+  </si>
+  <si>
     <t>2024-01-07 : Étape 5 copiée de 2023 avant modif étape Senneterre. À valider.</t>
   </si>
   <si>
+    <t>Gestion du circuit urbain - Ville / CO</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À MODIFIER </t>
+  </si>
+  <si>
     <t>Voie ferrée oblique à la route</t>
   </si>
   <si>
+    <t>Contrôle policier, intersection route provinciale</t>
+  </si>
+  <si>
+    <t>Contrôle policier, intersection secteur Cadillac</t>
+  </si>
+  <si>
     <t>Contrôle policier, intersection secteur Riviere-Heva</t>
   </si>
   <si>
     <t>Contrôle policier, intersection secteur Ch. Lac Malartic</t>
   </si>
   <si>
+    <t>Voie ferrée perpendiculaire à la route et début du terre-plein</t>
+  </si>
+  <si>
+    <t>Voie ferrée oblique à la route - Malartic</t>
+  </si>
+  <si>
     <t>Retressissment Ville de Malartic</t>
   </si>
   <si>
-    <t>sign_20</t>
-  </si>
-  <si>
-    <t>sign_21</t>
-  </si>
-  <si>
-    <t>sign_22</t>
-  </si>
-  <si>
     <t>sign_23</t>
   </si>
   <si>
@@ -548,195 +590,6 @@
   </si>
   <si>
     <t>Gestion dans rond-point - Signaleur et SQ pour traffic - tout à droite</t>
-  </si>
-  <si>
-    <t>Contrôle policier, intersection ch mine Westwood</t>
-  </si>
-  <si>
-    <t>Contrôle policier, intersection chemin Preissac</t>
-  </si>
-  <si>
-    <t>Contrôle policier, intersection secteur Cadillac (École)</t>
-  </si>
-  <si>
-    <t>Contrôle policier, intersection secteur Cadillac (Station-service)</t>
-  </si>
-  <si>
-    <t>Terre-Plein entrée rond point Malartic - tous à droite &lt;br/&gt;Série de cônes vers la direction droite</t>
-  </si>
-  <si>
-    <t>Voie ferrée - Malartic</t>
-  </si>
-  <si>
-    <t>Retressissment Ville de Malartic (Caisse)</t>
-  </si>
-  <si>
-    <t>Retressissment Ville de Malartic (Pétro)</t>
-  </si>
-  <si>
-    <t>Retressissment Ville de Malartic - terre-plein sortie ville</t>
-  </si>
-  <si>
-    <t>Retressissment Ville de Malartic - terre-plein av Hochelaga</t>
-  </si>
-  <si>
-    <t>Terre-plein Forest - Sabourin : tout à gauche</t>
-  </si>
-  <si>
-    <t>Bretelle Forest - Sabourin : tout à gauche - sens inverse</t>
-  </si>
-  <si>
-    <t>Bd Sabourin - Voie Est en sens inverse jusqu'à Des Pins</t>
-  </si>
-  <si>
-    <t>Intersection Des Pins direction voie Sud - séparation intersection en diagonale</t>
-  </si>
-  <si>
-    <t>Rampe de départ - voir croquis complet</t>
-  </si>
-  <si>
-    <t>Virage gauche - rue Allard - 2 sens - séparation</t>
-  </si>
-  <si>
-    <t>Virage droite - École - séparation 2 sens</t>
-  </si>
-  <si>
-    <t>Entrée - Sortie Moto suiveuse</t>
-  </si>
-  <si>
-    <t>Terre-plein - séparation voies Dennison - tout à droite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retour sur une seule voie </t>
-  </si>
-  <si>
-    <t>Virage à gauche - rue Self - 2 sens</t>
-  </si>
-  <si>
-    <t>Terre-plein - Self &amp; 7e - 2 sens dans la voie Sud</t>
-  </si>
-  <si>
-    <t>Intersection double sens Des Pins - Sabourin</t>
-  </si>
-  <si>
-    <t>Entrée - Sortie Stationnement pour demi Tour</t>
-  </si>
-  <si>
-    <t>Demi-Tour -- fond du stationnement roulotte</t>
-  </si>
-  <si>
-    <t>Terre-plein retour sur Rue Self</t>
-  </si>
-  <si>
-    <t>Zone décélération à protéger (voie de traverse des voitures)</t>
-  </si>
-  <si>
-    <t>Terre-plein</t>
-  </si>
-  <si>
-    <t>Légèrement à droite - Ch Lac Mourier</t>
-  </si>
-  <si>
-    <t>Légèrement à droite - Rivière-Héva &amp; Intersection Amos</t>
-  </si>
-  <si>
-    <t>Virage gauche - Rue La Sarre</t>
-  </si>
-  <si>
-    <t>Virage gauche - 117 / Royale</t>
-  </si>
-  <si>
-    <t>Contrôle Traffic 117 - Virage gauche rue Principale</t>
-  </si>
-  <si>
-    <t>Rétrécicement bollard protextion - signalisation pour protéger - Ville de RN</t>
-  </si>
-  <si>
-    <t>Rétrécicement troittoir rue des Pins - signalisation pour protéger</t>
-  </si>
-  <si>
-    <t>Voie ferré / Terre-plein - tous à droite</t>
-  </si>
-  <si>
-    <t>Intersection rue La Salle - tout droit</t>
-  </si>
-  <si>
-    <t>Virage en "S" vers Avenue d'Abitibi</t>
-  </si>
-  <si>
-    <t>Virage final à gauche - rue de la Paix</t>
-  </si>
-  <si>
-    <t>Zone déviation voitures suiveuses</t>
-  </si>
-  <si>
-    <t>Zone décélération jsuqu'à rue Hochelaga</t>
-  </si>
-  <si>
-    <t>Voie ferrée</t>
-  </si>
-  <si>
-    <t>Terre-plein après voie ferrée</t>
-  </si>
-  <si>
-    <t>Terre-plein, tout à droite (devant Centre du camping)</t>
-  </si>
-  <si>
-    <t>Terre-plein, tout à droite (devant AIM)</t>
-  </si>
-  <si>
-    <t>Terre-plein, tout à droite (devant pneu GBM)</t>
-  </si>
-  <si>
-    <t>Virage gauche,Contrôle policier, intersection route provinciale</t>
-  </si>
-  <si>
-    <t>Voie ferrée à angle</t>
-  </si>
-  <si>
-    <t>Contrôle policier, virage à droite sur route provinciale 386</t>
-  </si>
-  <si>
-    <t>Terre-Plein (Barraute, virage à gauche)</t>
-  </si>
-  <si>
-    <t>Terre-plein blvd JJ Cossette (tout à droite, après intersection du Portage)</t>
-  </si>
-  <si>
-    <t>Entrée carrefour giratoire 7e rue &amp; 117, (tout à droite)</t>
-  </si>
-  <si>
-    <t>Terre-plein intersection 7e &amp; 7e (tout à droite)</t>
-  </si>
-  <si>
-    <t>sign_32</t>
-  </si>
-  <si>
-    <t>sign_33</t>
-  </si>
-  <si>
-    <t>Entrée dans rond point - terre-plein</t>
-  </si>
-  <si>
-    <t>Terre-plein, tout à droite (devant Mazda)</t>
-  </si>
-  <si>
-    <t>sign_34</t>
-  </si>
-  <si>
-    <t>Terre-plein, tout à droite (devant cimetière)</t>
-  </si>
-  <si>
-    <t>Virage à gauche sur 4e rue ouest</t>
-  </si>
-  <si>
-    <t>Virage à droite par la bretelle</t>
-  </si>
-  <si>
-    <t>Contrôle policier, intersection route provinciale, virage à droite sur route 117</t>
-  </si>
-  <si>
-    <t>Terre-plein, tout à gauche et prendre première sortie à gauche</t>
   </si>
 </sst>
 </file>
@@ -1461,7 +1314,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1594,7 +1447,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>56</v>
@@ -1789,10 +1642,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59035EEC-8A2E-CE47-A69A-0CAB24334359}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1840,7 +1693,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
@@ -1863,7 +1716,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
         <v>56</v>
@@ -1886,7 +1739,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
@@ -1909,7 +1762,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
@@ -1931,7 +1784,7 @@
       <c r="C6" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>159</v>
       </c>
       <c r="E6" t="s">
@@ -1954,7 +1807,7 @@
       <c r="C7" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>160</v>
       </c>
       <c r="E7" t="s">
@@ -1977,8 +1830,8 @@
       <c r="C8" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>161</v>
+      <c r="D8" t="s">
+        <v>160</v>
       </c>
       <c r="E8" t="s">
         <v>64</v>
@@ -2001,7 +1854,7 @@
         <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
@@ -2010,7 +1863,7 @@
         <v>74</v>
       </c>
       <c r="G9" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
@@ -2024,7 +1877,7 @@
         <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -2033,7 +1886,7 @@
         <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
@@ -2047,16 +1900,16 @@
         <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F11" t="s">
         <v>74</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
@@ -2070,7 +1923,7 @@
         <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="E12" t="s">
         <v>64</v>
@@ -2079,7 +1932,7 @@
         <v>74</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
@@ -2092,17 +1945,17 @@
       <c r="C13" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>162</v>
+      <c r="D13" t="s">
+        <v>163</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
@@ -2116,7 +1969,7 @@
         <v>96</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="E14" t="s">
         <v>64</v>
@@ -2125,7 +1978,7 @@
         <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
@@ -2138,8 +1991,8 @@
       <c r="C15" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>163</v>
+      <c r="D15" t="s">
+        <v>164</v>
       </c>
       <c r="E15" t="s">
         <v>56</v>
@@ -2161,7 +2014,7 @@
       <c r="C16" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" t="s">
         <v>165</v>
       </c>
       <c r="E16" t="s">
@@ -2179,22 +2032,22 @@
         <v>58</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>166</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
@@ -2202,22 +2055,22 @@
         <v>58</v>
       </c>
       <c r="B18">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>168</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="G18" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
@@ -2225,184 +2078,44 @@
         <v>58</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>164</v>
+        <v>169</v>
+      </c>
+      <c r="D19" t="s">
+        <v>170</v>
       </c>
       <c r="E19" t="s">
         <v>64</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="G19" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" t="s">
-        <v>148</v>
-      </c>
-      <c r="E20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" t="s">
-        <v>71</v>
-      </c>
+      <c r="A20" s="10"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>149</v>
-      </c>
-      <c r="D21" t="s">
-        <v>148</v>
-      </c>
-      <c r="E21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" t="s">
-        <v>71</v>
-      </c>
+      <c r="A21" s="10"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>150</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E22" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" t="s">
-        <v>71</v>
-      </c>
+      <c r="A22" s="10"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>151</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" t="s">
-        <v>71</v>
-      </c>
+      <c r="A23" s="10"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>152</v>
-      </c>
-      <c r="D24" t="s">
-        <v>153</v>
-      </c>
-      <c r="E24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" t="s">
-        <v>56</v>
-      </c>
+      <c r="A24" s="10"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>154</v>
-      </c>
-      <c r="D25" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" t="s">
-        <v>55</v>
-      </c>
+      <c r="A25" s="10"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>155</v>
-      </c>
-      <c r="D26" t="s">
-        <v>156</v>
-      </c>
-      <c r="E26" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" t="s">
-        <v>55</v>
-      </c>
+      <c r="A26" s="10"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="10"/>
@@ -2427,27 +2140,6 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" s="10"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A35" s="10"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A36" s="10"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A37" s="10"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A38" s="10"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A39" s="10"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A40" s="10"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A41" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -2482,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4800E175-391C-4882-AD71-91732BA4C7F2}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2533,546 +2225,63 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>199</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" t="s">
-        <v>66</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" t="s">
-        <v>66</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="2">
-        <v>34</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" t="s">
-        <v>202</v>
-      </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" t="s">
-        <v>203</v>
-      </c>
-      <c r="E12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" t="s">
-        <v>204</v>
-      </c>
-      <c r="E13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" t="s">
-        <v>66</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" t="s">
-        <v>205</v>
-      </c>
-      <c r="E14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" t="s">
-        <v>56</v>
-      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" t="s">
-        <v>206</v>
-      </c>
-      <c r="E15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" t="s">
-        <v>54</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" t="s">
-        <v>207</v>
-      </c>
-      <c r="E16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="5">
-        <v>13</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" t="s">
-        <v>207</v>
-      </c>
-      <c r="E17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="5">
-        <v>14</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="5">
-        <v>15</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" t="s">
-        <v>208</v>
-      </c>
-      <c r="E19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="5">
-        <v>16</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="5">
-        <v>17</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="5">
-        <v>18</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D22" t="s">
-        <v>209</v>
-      </c>
-      <c r="E22" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="5">
-        <v>19</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24">
-        <v>20</v>
-      </c>
-      <c r="C24" t="s">
-        <v>149</v>
-      </c>
-      <c r="D24" t="s">
-        <v>199</v>
-      </c>
-      <c r="E24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25">
-        <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>150</v>
-      </c>
-      <c r="D25" t="s">
-        <v>210</v>
-      </c>
-      <c r="E25" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" t="s">
-        <v>67</v>
-      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -3080,24 +2289,24 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7BB46DD1-CE67-8840-86C9-A7B4DD4EA804}">
           <x14:formula1>
             <xm:f>Lexique!$D$2:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>E14:E1048576 E2:E13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B2F24BC-BBE5-3242-8C11-39321438202A}">
           <x14:formula1>
             <xm:f>Lexique!$E$2:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>F14:F1048576 F2:F13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2AB93EB3-1866-E243-98C3-B11D12762F37}">
           <x14:formula1>
             <xm:f>Lexique!$F$2:$F$17</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
+          <xm:sqref>G14:G1048576 G2:G13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3107,21 +2316,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB129F3F-5845-E94C-BB9B-41541692CC0D}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.5" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -3151,7 +2360,7 @@
       <c r="A2" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="str">
@@ -3159,7 +2368,7 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>172</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
         <v>65</v>
@@ -3167,199 +2376,119 @@
       <c r="F2" t="s">
         <v>73</v>
       </c>
-      <c r="G2" t="s">
-        <v>67</v>
+      <c r="G2" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="str">
+      <c r="A3" t="str">
         <f>A2</f>
         <v>E3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f t="shared" ref="C3:C4" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <f t="shared" ref="C3:C10" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
         <v>sign_02</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>173</v>
+        <v>119</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="str">
-        <f t="shared" ref="A4:A16" si="1">A3</f>
-        <v>E3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="str">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <f t="shared" ref="A8:A10" si="1">A7</f>
+        <v>0</v>
+      </c>
+      <c r="B8" s="5">
+        <v>90</v>
+      </c>
+      <c r="C8" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>sign_03</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E4" t="s">
+        <v>sign_90</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" t="s">
         <v>65</v>
       </c>
-      <c r="F4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="8" t="str">
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9">
         <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <f t="shared" ref="C5:C15" si="2">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B5,"0#"))</f>
-        <v>sign_04</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="5">
+        <v>91</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_91</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
         <v>73</v>
       </c>
-      <c r="G5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="str">
+      <c r="G9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10">
         <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>sign_05</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>sign_06</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>sign_07</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>sign_08</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="B10" s="5">
+        <v>92</v>
       </c>
       <c r="C10" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>sign_09</v>
+        <f t="shared" si="0"/>
+        <v>sign_92</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>180</v>
+        <v>122</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -3368,158 +2497,32 @@
         <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>sign_10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" t="s">
-        <v>67</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>sign_11</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" t="s">
-        <v>67</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>sign_12</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" t="s">
-        <v>55</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>sign_13</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" t="s">
-        <v>67</v>
-      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B15">
-        <v>15</v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>sign_15</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" t="s">
-        <v>67</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>E3</v>
-      </c>
-      <c r="B16">
-        <v>14</v>
-      </c>
-      <c r="C16" s="5" t="str">
-        <f t="shared" ref="C16" si="3">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B16,"0#"))</f>
-        <v>sign_14</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" t="s">
-        <v>67</v>
-      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B17" s="5"/>
@@ -3528,42 +2531,6 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3575,19 +2542,19 @@
           <x14:formula1>
             <xm:f>Lexique!$D$2:$D$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E27</xm:sqref>
+          <xm:sqref>E2:E10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CADB21EB-5FBA-F948-91A8-13DA27ECCDDC}">
           <x14:formula1>
             <xm:f>Lexique!$E$2:$E$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F27</xm:sqref>
+          <xm:sqref>F2:F10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{446A4710-3B5A-9247-B67D-D204A01F91E2}">
           <x14:formula1>
             <xm:f>Lexique!$F$2:$F$13</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G27</xm:sqref>
+          <xm:sqref>G3:G10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3597,16 +2564,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F06BA10-C7CB-D34A-A68E-94110B0F7625}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="62.5" customWidth="1"/>
     <col min="5" max="7" width="15.6640625" customWidth="1"/>
@@ -3637,626 +2604,360 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
-        <v>sign_01</v>
+      <c r="C2" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
-        <v>134</v>
+      <c r="A3" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="str">
-        <f t="shared" ref="C3:C24" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
-        <v>sign_02</v>
+      <c r="C3" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G3" t="s">
-        <v>55</v>
+      <c r="G3" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="13" t="s">
-        <v>134</v>
+      <c r="A4" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_03</v>
+      <c r="C4" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>185</v>
+        <v>141</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="13" t="s">
-        <v>134</v>
+      <c r="A5" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_04</v>
+      <c r="C5" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>185</v>
+        <v>142</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="13" t="s">
-        <v>134</v>
+      <c r="A6" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_06</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="2">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_07</v>
+      <c r="C7" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="2">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_09</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="F13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="2">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="2">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="G13" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_05</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B12" s="2">
-        <v>13</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_13</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="G14" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="B15" s="2">
         <v>14</v>
       </c>
-      <c r="C13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_14</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="C15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="G15" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="2">
         <v>15</v>
       </c>
-      <c r="C14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_15</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="C16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="13" t="str">
-        <f>A14</f>
-        <v>E4</v>
-      </c>
-      <c r="B15" s="5">
-        <v>8</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_08</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="13" t="str">
-        <f t="shared" ref="A16:A24" si="1">A15</f>
-        <v>E4</v>
-      </c>
-      <c r="B16" s="5">
-        <v>16</v>
-      </c>
-      <c r="C16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>186</v>
-      </c>
-      <c r="E16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="B17">
-        <v>20</v>
-      </c>
-      <c r="C17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>142</v>
-      </c>
-      <c r="E17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="G16" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="B18">
-        <v>21</v>
-      </c>
-      <c r="C18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_21</v>
-      </c>
-      <c r="D18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="B19">
-        <v>22</v>
-      </c>
-      <c r="C19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_22</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="B20">
-        <v>23</v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_23</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="B21">
-        <v>24</v>
-      </c>
-      <c r="C21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_24</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="B22">
-        <v>25</v>
-      </c>
-      <c r="C22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_25</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E22" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="B23">
-        <v>26</v>
-      </c>
-      <c r="C23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_26</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="B24">
-        <v>27</v>
-      </c>
-      <c r="C24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_27</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E24" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="13"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="13"/>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="13"/>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C28" s="2"/>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C6514F4A-BD79-DB46-A0BE-57501B73CBDD}">
-          <x14:formula1>
-            <xm:f>Lexique!$F$2:$F$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>G8 G3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{463BCA35-24F0-AE4C-9B9D-BD2295FAB2D2}">
-          <x14:formula1>
-            <xm:f>Lexique!$E$2:$E$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>F8 F3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCABF94A-CF6E-0142-A54D-4679177E7DC0}">
-          <x14:formula1>
-            <xm:f>Lexique!$D$2:$D$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>E8 E3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B510EDD3-1D60-2C4F-BC8F-8A16F0CAE8D8}">
-          <x14:formula1>
-            <xm:f>Lexique!$F$2:$F$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>G18:G41</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4754FE9-959E-5446-A32D-C448446ADFA1}">
-          <x14:formula1>
-            <xm:f>Lexique!$E$2:$E$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>F18:F41</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{55D5426C-BF6C-674D-B316-A5FC9600E4BB}">
-          <x14:formula1>
-            <xm:f>Lexique!$D$2:$D$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>E18:E41</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4304,7 +3005,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -4313,7 +3014,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
@@ -4327,7 +3028,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -4336,7 +3037,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>56</v>
@@ -4350,7 +3051,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -4359,7 +3060,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>64</v>
@@ -4373,7 +3074,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -4396,7 +3097,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -4419,7 +3120,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -4442,7 +3143,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -4465,7 +3166,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -4488,7 +3189,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -4497,7 +3198,7 @@
         <v>101</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>56</v>
@@ -4511,7 +3212,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -4520,7 +3221,7 @@
         <v>114</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>65</v>
@@ -4529,12 +3230,12 @@
         <v>73</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -4543,7 +3244,7 @@
         <v>115</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>65</v>
@@ -4552,12 +3253,12 @@
         <v>73</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -4566,7 +3267,7 @@
         <v>102</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>64</v>
@@ -4580,7 +3281,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -4603,7 +3304,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -4612,7 +3313,7 @@
         <v>97</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>64</v>
@@ -4626,7 +3327,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -4635,7 +3336,7 @@
         <v>98</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>64</v>
@@ -4649,7 +3350,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
@@ -4658,7 +3359,7 @@
         <v>99</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>64</v>
@@ -4672,7 +3373,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -4681,7 +3382,7 @@
         <v>100</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>64</v>
@@ -4695,7 +3396,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
@@ -4704,7 +3405,7 @@
         <v>116</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>64</v>
@@ -4718,7 +3419,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
@@ -4727,7 +3428,7 @@
         <v>117</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>64</v>
@@ -4741,16 +3442,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B21" s="2">
         <v>50</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>64</v>
@@ -4764,16 +3465,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B22" s="2">
         <v>51</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>64</v>
@@ -4787,16 +3488,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B23" s="2">
         <v>60</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>56</v>
@@ -4830,8 +3531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DA1B73-E162-C44F-BFAF-F0B7401711F0}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4869,119 +3570,56 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>118</v>
+      <c r="A2" s="8" t="s">
+        <v>123</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>92</v>
+      <c r="C2" s="5" t="str">
+        <f t="shared" ref="C2" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7" s="2"/>
@@ -5093,7 +3731,7 @@
           <x14:formula1>
             <xm:f>Lexique!$F$2:$F$17</xm:f>
           </x14:formula1>
-          <xm:sqref>G7:G18</xm:sqref>
+          <xm:sqref>G2:G18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5105,8 +3743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F8F1C6-7AEF-9949-BBA2-37380A45C53E}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5150,11 +3788,12 @@
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>92</v>
+      <c r="C2" s="5" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>217</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
@@ -5167,234 +3806,44 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
-      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="5">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" t="s">
-        <v>219</v>
-      </c>
-      <c r="E4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" t="s">
-        <v>66</v>
-      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>56</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="5">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" t="s">
-        <v>87</v>
-      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="5">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" t="s">
-        <v>67</v>
-      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" s="5">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" t="s">
-        <v>67</v>
-      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="5">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" t="s">
-        <v>220</v>
-      </c>
-      <c r="E9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" t="s">
-        <v>67</v>
-      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="5">
-        <v>9</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" t="s">
-        <v>87</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" s="5">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" t="s">
-        <v>67</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" s="5">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D12" t="s">
-        <v>210</v>
-      </c>
-      <c r="E12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" t="s">
-        <v>56</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>

</xml_diff>